<commit_message>
Minor fixes to test, application, and cylinder setup
</commit_message>
<xml_diff>
--- a/Pinouts.xlsx
+++ b/Pinouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Type</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>22 awg</t>
+  </si>
+  <si>
+    <t>Tote Intake Sensor</t>
+  </si>
+  <si>
+    <t>Ejector Out</t>
+  </si>
+  <si>
+    <t>Ejector In</t>
   </si>
 </sst>
 </file>
@@ -201,10 +210,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -219,12 +229,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D23" totalsRowShown="0">
-  <autoFilter ref="A1:D23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D26" totalsRowShown="0">
+  <autoFilter ref="A1:D26"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Use"/>
     <tableColumn id="2" name="Type"/>
@@ -559,19 +574,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="5.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -585,7 +601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -600,7 +616,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -615,7 +631,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -630,7 +646,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -645,7 +661,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -660,7 +676,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -675,7 +691,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -690,7 +706,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -705,7 +721,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -720,7 +736,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -735,7 +751,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -750,7 +766,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -765,7 +781,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -780,7 +796,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -795,7 +811,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -810,7 +826,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -825,7 +841,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -840,7 +856,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -855,7 +871,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -870,7 +886,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -885,7 +901,7 @@
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -893,23 +909,68 @@
         <v>25</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>RoboRio</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f>IF(EXACT(B23,"Analog"),IF(C23&lt;4,"RoboRio","MXP"),IF(EXACT(B23,"Digital"),IF(C23&lt;10,"RoboRio","MXP"),IF(EXACT(B23,"PWM"),IF(C23&lt;10,"RoboRio","MXP"),"N/A")))</f>
+        <v>RoboRio</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f>IF(EXACT(B24,"Analog"),IF(C24&lt;4,"RoboRio","MXP"),IF(EXACT(B24,"Digital"),IF(C24&lt;10,"RoboRio","MXP"),IF(EXACT(B24,"PWM"),IF(C24&lt;10,"RoboRio","MXP"),"N/A")))</f>
+        <v>RoboRio</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f>IF(EXACT(B25,"Analog"),IF(C25&lt;4,"RoboRio","MXP"),IF(EXACT(B25,"Digital"),IF(C25&lt;10,"RoboRio","MXP"),IF(EXACT(B25,"PWM"),IF(C25&lt;10,"RoboRio","MXP"),"N/A")))</f>
+        <v>RoboRio</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C26" s="1">
         <v>0</v>
       </c>
-      <c r="D23" s="2" t="str">
-        <f>IF(EXACT(B23,"Analog"),IF(C23&lt;4,"RoboRio","MXP"),IF(EXACT(B23,"Digital"),IF(C23&lt;10,"RoboRio","MXP"),IF(EXACT(B23,"PWM"),IF(C23&lt;10,"RoboRio","MXP"),"N/A")))</f>
+      <c r="D26" s="2" t="str">
+        <f>IF(EXACT(B26,"Analog"),IF(C26&lt;4,"RoboRio","MXP"),IF(EXACT(B26,"Digital"),IF(C26&lt;10,"RoboRio","MXP"),IF(EXACT(B26,"PWM"),IF(C26&lt;10,"RoboRio","MXP"),"N/A")))</f>
         <v>N/A</v>
       </c>
     </row>
@@ -935,12 +996,12 @@
       <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -948,7 +1009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -956,7 +1017,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -964,7 +1025,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -972,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -980,7 +1041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -988,7 +1049,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -996,7 +1057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>

</xml_diff>